<commit_message>
Had FAMM2 (THETA) Round the wrong way
</commit_message>
<xml_diff>
--- a/Traps.xlsx
+++ b/Traps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="33">
   <si>
     <t>a</t>
   </si>
@@ -95,9 +95,6 @@
     <t xml:space="preserve">Means: </t>
   </si>
   <si>
-    <t>FAMM</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
@@ -114,6 +111,18 @@
   </si>
   <si>
     <t>https://plot.ly/create/</t>
+  </si>
+  <si>
+    <t>X FAMM</t>
+  </si>
+  <si>
+    <t>THETA FAMM</t>
+  </si>
+  <si>
+    <t>FAMM2</t>
+  </si>
+  <si>
+    <t>FAMM1</t>
   </si>
 </sst>
 </file>
@@ -495,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +515,7 @@
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +526,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -525,8 +534,11 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +546,7 @@
         <v>-2.4</v>
       </c>
       <c r="C2" s="1">
-        <v>-1.8</v>
+        <v>-2.4</v>
       </c>
       <c r="D2" s="1">
         <v>-0.7</v>
@@ -543,16 +555,53 @@
         <v>0.4</v>
       </c>
       <c r="F2" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2">
+        <v>2</v>
+      </c>
+      <c r="X2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -560,7 +609,7 @@
         <v>-2.4</v>
       </c>
       <c r="C3" s="1">
-        <v>-1.5</v>
+        <v>-2</v>
       </c>
       <c r="D3" s="1">
         <v>-0.4</v>
@@ -569,18 +618,55 @@
         <v>0.7</v>
       </c>
       <c r="F3" s="1">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>8</v>
+      </c>
+      <c r="V3" s="3">
+        <v>7</v>
+      </c>
+      <c r="W3" s="3">
+        <v>6</v>
+      </c>
+      <c r="X3" s="3">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>-1.8</v>
+        <v>-2.4</v>
       </c>
       <c r="C4" s="1">
         <v>-0.7</v>
@@ -589,7 +675,7 @@
         <v>0.4</v>
       </c>
       <c r="E4" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1">
         <v>2.4</v>
@@ -597,13 +683,50 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3">
+        <v>7</v>
+      </c>
+      <c r="V4" s="3">
+        <v>6</v>
+      </c>
+      <c r="W4" s="3">
+        <v>5</v>
+      </c>
+      <c r="X4" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-1.5</v>
+        <v>-2</v>
       </c>
       <c r="C5" s="1">
         <v>-0.4</v>
@@ -612,7 +735,7 @@
         <v>0.7</v>
       </c>
       <c r="E5" s="1">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="F5" s="1">
         <v>2.4</v>
@@ -620,8 +743,86 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2</v>
+      </c>
+      <c r="U5" s="3">
+        <v>6</v>
+      </c>
+      <c r="V5" s="3">
+        <v>5</v>
+      </c>
+      <c r="W5" s="3">
+        <v>4</v>
+      </c>
+      <c r="X5" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="M6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="2">
+        <v>3</v>
+      </c>
+      <c r="U6" s="3">
+        <v>5</v>
+      </c>
+      <c r="V6" s="3">
+        <v>4</v>
+      </c>
+      <c r="W6" s="3">
+        <v>3</v>
+      </c>
+      <c r="X6" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -632,7 +833,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -640,8 +841,45 @@
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="3"/>
+      <c r="T7" s="2">
+        <v>4</v>
+      </c>
+      <c r="U7" s="3">
+        <v>4</v>
+      </c>
+      <c r="V7" s="3">
+        <v>3</v>
+      </c>
+      <c r="W7" s="3">
+        <v>2</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +887,7 @@
         <v>-4.5</v>
       </c>
       <c r="C8" s="1">
-        <v>-2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="D8" s="1">
         <v>-1</v>
@@ -658,13 +896,16 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -672,7 +913,7 @@
         <v>-4.5</v>
       </c>
       <c r="C9" s="1">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="D9" s="1">
         <v>-0.5</v>
@@ -681,18 +922,55 @@
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2">
+        <v>2</v>
+      </c>
+      <c r="X9" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1">
-        <v>-2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="C10" s="1">
         <v>-1</v>
@@ -701,7 +979,7 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1">
         <v>4.5</v>
@@ -709,13 +987,50 @@
       <c r="G10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
+        <v>1</v>
+      </c>
+      <c r="W10" s="3">
+        <v>2</v>
+      </c>
+      <c r="X10" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="1">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="C11" s="1">
         <v>-0.5</v>
@@ -724,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="F11" s="1">
         <v>4.5</v>
@@ -732,8 +1047,86 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S11" s="3"/>
+      <c r="T11" s="2">
+        <v>1</v>
+      </c>
+      <c r="U11" s="3">
+        <v>1</v>
+      </c>
+      <c r="V11" s="3">
+        <v>2</v>
+      </c>
+      <c r="W11" s="3">
+        <v>3</v>
+      </c>
+      <c r="X11" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="M12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="2">
+        <v>2</v>
+      </c>
+      <c r="U12" s="3">
+        <v>2</v>
+      </c>
+      <c r="V12" s="3">
+        <v>3</v>
+      </c>
+      <c r="W12" s="3">
+        <v>4</v>
+      </c>
+      <c r="X12" s="3">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -744,7 +1137,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
@@ -752,8 +1145,45 @@
       <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="2">
+        <v>3</v>
+      </c>
+      <c r="U13" s="3">
+        <v>3</v>
+      </c>
+      <c r="V13" s="3">
+        <v>4</v>
+      </c>
+      <c r="W13" s="3">
+        <v>5</v>
+      </c>
+      <c r="X13" s="3">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,7 +1191,7 @@
         <v>-0.8</v>
       </c>
       <c r="C14" s="1">
-        <v>-0.55000000000000004</v>
+        <v>-0.8</v>
       </c>
       <c r="D14" s="1">
         <v>-0.2</v>
@@ -770,13 +1200,50 @@
         <v>0.1</v>
       </c>
       <c r="F14" s="1">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S14" s="3"/>
+      <c r="T14" s="2">
+        <v>4</v>
+      </c>
+      <c r="U14" s="3">
+        <v>4</v>
+      </c>
+      <c r="V14" s="3">
+        <v>5</v>
+      </c>
+      <c r="W14" s="3">
+        <v>6</v>
+      </c>
+      <c r="X14" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -784,7 +1251,7 @@
         <v>-0.8</v>
       </c>
       <c r="C15" s="1">
-        <v>-0.4</v>
+        <v>-0.7</v>
       </c>
       <c r="D15" s="1">
         <v>-0.1</v>
@@ -793,18 +1260,18 @@
         <v>0.2</v>
       </c>
       <c r="F15" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="C16" s="1">
         <v>-0.2</v>
@@ -813,7 +1280,7 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="1">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="F16" s="1">
         <v>0.8</v>
@@ -822,12 +1289,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1">
-        <v>-0.4</v>
+        <v>-0.7</v>
       </c>
       <c r="C17" s="1">
         <v>-0.1</v>
@@ -836,7 +1303,7 @@
         <v>0.2</v>
       </c>
       <c r="E17" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="F17" s="1">
         <v>0.8</v>
@@ -845,12 +1312,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -861,7 +1328,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>7</v>
@@ -870,7 +1337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,7 +1345,7 @@
         <v>-0.4</v>
       </c>
       <c r="C20" s="1">
-        <v>-0.3</v>
+        <v>-0.4</v>
       </c>
       <c r="D20" s="1">
         <v>-0.1</v>
@@ -887,13 +1354,13 @@
         <v>0.05</v>
       </c>
       <c r="F20" s="1">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -901,7 +1368,7 @@
         <v>-0.4</v>
       </c>
       <c r="C21" s="1">
-        <v>-0.25</v>
+        <v>-0.35</v>
       </c>
       <c r="D21" s="1">
         <v>-0.05</v>
@@ -910,18 +1377,18 @@
         <v>0.1</v>
       </c>
       <c r="F21" s="1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>-0.3</v>
+        <v>-0.4</v>
       </c>
       <c r="C22" s="1">
         <v>-0.1</v>
@@ -930,7 +1397,7 @@
         <v>0.05</v>
       </c>
       <c r="E22" s="1">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="F22" s="1">
         <v>0.4</v>
@@ -939,12 +1406,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1">
-        <v>-0.2</v>
+        <v>-0.35</v>
       </c>
       <c r="C23" s="1">
         <v>-0.05</v>
@@ -953,248 +1420,12 @@
         <v>0.1</v>
       </c>
       <c r="E23" s="1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F23" s="1">
         <v>0.4</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>1</v>
-      </c>
-      <c r="K25" s="2">
-        <v>2</v>
-      </c>
-      <c r="L25" s="2">
-        <v>3</v>
-      </c>
-      <c r="M25" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
-        <v>8</v>
-      </c>
-      <c r="J26" s="3">
-        <v>7</v>
-      </c>
-      <c r="K26" s="3">
-        <v>6</v>
-      </c>
-      <c r="L26" s="3">
-        <v>5</v>
-      </c>
-      <c r="M26" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3">
-        <v>7</v>
-      </c>
-      <c r="J27" s="3">
-        <v>6</v>
-      </c>
-      <c r="K27" s="3">
-        <v>5</v>
-      </c>
-      <c r="L27" s="3">
-        <v>4</v>
-      </c>
-      <c r="M27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="2">
-        <v>2</v>
-      </c>
-      <c r="I28" s="3">
-        <v>6</v>
-      </c>
-      <c r="J28" s="3">
-        <v>5</v>
-      </c>
-      <c r="K28" s="3">
-        <v>4</v>
-      </c>
-      <c r="L28" s="3">
-        <v>3</v>
-      </c>
-      <c r="M28" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="2">
-        <v>3</v>
-      </c>
-      <c r="I29" s="3">
-        <v>5</v>
-      </c>
-      <c r="J29" s="3">
-        <v>4</v>
-      </c>
-      <c r="K29" s="3">
-        <v>3</v>
-      </c>
-      <c r="L29" s="3">
-        <v>2</v>
-      </c>
-      <c r="M29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="2">
-        <v>4</v>
-      </c>
-      <c r="I30" s="3">
-        <v>4</v>
-      </c>
-      <c r="J30" s="3">
-        <v>3</v>
-      </c>
-      <c r="K30" s="3">
-        <v>2</v>
-      </c>
-      <c r="L30" s="3">
-        <v>1</v>
-      </c>
-      <c r="M30" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Using Yamakawa's method instead of the 2 FAMM approach
</commit_message>
<xml_diff>
--- a/Traps.xlsx
+++ b/Traps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="39">
   <si>
     <t>a</t>
   </si>
@@ -123,6 +123,24 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>YAMAKAWAWAWA</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>YAMAKAWAWAWAW FAMM</t>
+  </si>
+  <si>
+    <t>FAMM3</t>
+  </si>
+  <si>
+    <t>ANGLE</t>
+  </si>
+  <si>
+    <t>POSITION</t>
   </si>
 </sst>
 </file>
@@ -175,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +205,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -504,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1191,16 +1212,16 @@
         <v>-0.8</v>
       </c>
       <c r="C14" s="1">
-        <v>-0.6</v>
+        <v>-0.7</v>
       </c>
       <c r="D14" s="1">
         <v>-0.1</v>
       </c>
       <c r="E14" s="1">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1289,21 +1310,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1">
-        <v>-0.5</v>
+        <v>-0.4</v>
       </c>
       <c r="C17" s="1">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
         <v>0.1</v>
       </c>
       <c r="E17" s="1">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="F17" s="1">
         <v>0.8</v>
@@ -1312,12 +1333,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1337,7 +1358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1383,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1406,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1427,6 +1448,282 @@
       </c>
       <c r="G23" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <v>-4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>4</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits to make it a bit easier to read
</commit_message>
<xml_diff>
--- a/Traps.xlsx
+++ b/Traps.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:G30"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1514,7 @@
         <v>-0.5</v>
       </c>
       <c r="E27" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1634,7 +1634,7 @@
         <v>-1</v>
       </c>
       <c r="C30" s="1">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
         <v>0.5</v>

</xml_diff>

<commit_message>
Slight change to make it a bit faster
</commit_message>
<xml_diff>
--- a/Traps.xlsx
+++ b/Traps.xlsx
@@ -526,14 +526,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="34.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -1741,7 +1741,7 @@
         <v>-0.2</v>
       </c>
       <c r="D34" s="1">
-        <v>0</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="E34" s="1">
         <v>0.15</v>
@@ -1764,7 +1764,7 @@
         <v>-0.15</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E35" s="1">
         <v>0.2</v>

</xml_diff>